<commit_message>
New updates on Java class and Object
</commit_message>
<xml_diff>
--- a/2024FEB_M1.xlsx
+++ b/2024FEB_M1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>S.N.</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t>Java inputs : String and Integer</t>
+  </si>
+  <si>
+    <t>Prajatantra diwas</t>
+  </si>
+  <si>
+    <t>Class and Object</t>
   </si>
 </sst>
 </file>
@@ -559,7 +565,9 @@
       <c r="B9" s="8">
         <v>45341</v>
       </c>
-      <c r="C9" s="9"/>
+      <c r="C9" s="9" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="7">
@@ -568,7 +576,9 @@
       <c r="B10" s="8">
         <v>45342</v>
       </c>
-      <c r="C10" s="9"/>
+      <c r="C10" s="9" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="7">
@@ -651,7 +661,7 @@
       </c>
       <c r="C19" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="20.25">
       <c r="A20" s="7">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Inheritace with classwork solution
</commit_message>
<xml_diff>
--- a/2024FEB_M1.xlsx
+++ b/2024FEB_M1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>S.N.</t>
   </si>
@@ -82,10 +82,16 @@
     <t>Leave, External Examiner</t>
   </si>
   <si>
+    <t>Shivaratri : Holiday</t>
+  </si>
+  <si>
     <t>Sarurday : Holiday</t>
   </si>
   <si>
     <t>Inheritance</t>
+  </si>
+  <si>
+    <t>Gyalpo Lhosar : Holiday</t>
   </si>
 </sst>
 </file>
@@ -803,7 +809,7 @@
         <v>45359</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
@@ -814,7 +820,7 @@
         <v>45360</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
@@ -825,7 +831,7 @@
         <v>45361</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
@@ -835,7 +841,9 @@
       <c r="B30" s="8">
         <v>45362</v>
       </c>
-      <c r="C30" s="9"/>
+      <c r="C30" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="7">

</xml_diff>

<commit_message>
Inheritance and interface in java
</commit_message>
<xml_diff>
--- a/2024FEB_M1.xlsx
+++ b/2024FEB_M1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>S.N.</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>Gyalpo Lhosar : Holiday</t>
+  </si>
+  <si>
+    <t>Inheritance and Interface</t>
   </si>
 </sst>
 </file>
@@ -852,7 +855,9 @@
       <c r="B31" s="8">
         <v>45363</v>
       </c>
-      <c r="C31" s="9"/>
+      <c r="C31" s="9" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="7">

</xml_diff>

<commit_message>
Interface and Method Overriding
</commit_message>
<xml_diff>
--- a/2024FEB_M1.xlsx
+++ b/2024FEB_M1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>S.N.</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>Inheritance and Interface</t>
+  </si>
+  <si>
+    <t>Interface and Method Overriding</t>
   </si>
 </sst>
 </file>
@@ -866,7 +869,9 @@
       <c r="B32" s="8">
         <v>45364</v>
       </c>
-      <c r="C32" s="9"/>
+      <c r="C32" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
       <c r="A33" s="7">

</xml_diff>

<commit_message>
Overriding and final keyword
</commit_message>
<xml_diff>
--- a/2024FEB_M1.xlsx
+++ b/2024FEB_M1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>S.N.</t>
   </si>
@@ -98,6 +98,15 @@
   </si>
   <si>
     <t>Interface and Method Overriding</t>
+  </si>
+  <si>
+    <t>1 - 4 Only</t>
+  </si>
+  <si>
+    <t>Holiday Saturday</t>
+  </si>
+  <si>
+    <t>Overriding and Final Keyword with Variable, mathod and class</t>
   </si>
 </sst>
 </file>
@@ -880,7 +889,9 @@
       <c r="B33" s="8">
         <v>45365</v>
       </c>
-      <c r="C33" s="9"/>
+      <c r="C33" s="9" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
       <c r="A34" s="7">
@@ -889,7 +900,9 @@
       <c r="B34" s="8">
         <v>45366</v>
       </c>
-      <c r="C34" s="9"/>
+      <c r="C34" s="9" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
       <c r="A35" s="7">
@@ -898,7 +911,9 @@
       <c r="B35" s="8">
         <v>45367</v>
       </c>
-      <c r="C35" s="9"/>
+      <c r="C35" s="9" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
       <c r="A36" s="7">
@@ -907,7 +922,9 @@
       <c r="B36" s="8">
         <v>45368</v>
       </c>
-      <c r="C36" s="9"/>
+      <c r="C36" s="9" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
       <c r="A37" s="7">

</xml_diff>

<commit_message>
Final keyword and access specifiers
</commit_message>
<xml_diff>
--- a/2024FEB_M1.xlsx
+++ b/2024FEB_M1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>S.N.</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>Overriding and Final Keyword with Variable, mathod and class</t>
+  </si>
+  <si>
+    <t>Final Keword and Access Specifiers</t>
   </si>
 </sst>
 </file>
@@ -933,7 +936,9 @@
       <c r="B37" s="8">
         <v>45369</v>
       </c>
-      <c r="C37" s="9"/>
+      <c r="C37" s="9" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
       <c r="A38" s="7">

</xml_diff>

<commit_message>
Thread Priority and Assignment One
</commit_message>
<xml_diff>
--- a/2024FEB_M1.xlsx
+++ b/2024FEB_M1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>S.N.</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>Threads</t>
+  </si>
+  <si>
+    <t>Threads Priority, Assignment assigned</t>
   </si>
 </sst>
 </file>
@@ -1036,7 +1039,9 @@
       <c r="B45" s="8">
         <v>45377</v>
       </c>
-      <c r="C45" s="9"/>
+      <c r="C45" s="9" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
       <c r="A46" s="7">

</xml_diff>

<commit_message>
Threads and Character streams
</commit_message>
<xml_diff>
--- a/2024FEB_M1.xlsx
+++ b/2024FEB_M1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>S.N.</t>
   </si>
@@ -125,6 +125,15 @@
   </si>
   <si>
     <t>Threads Priority, Assignment assigned</t>
+  </si>
+  <si>
+    <t>Threads group, Multithreading and Thread Call</t>
+  </si>
+  <si>
+    <t>Saturday Holiday</t>
+  </si>
+  <si>
+    <t>Stream Classes, Character Stream, BufferedReader</t>
   </si>
 </sst>
 </file>
@@ -545,7 +554,7 @@
   <cols>
     <col min="1" max="1" style="10" width="4.576428571428571" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="11" width="28.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="38.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="12" width="46.14785714285715" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -1050,7 +1059,9 @@
       <c r="B46" s="8">
         <v>45378</v>
       </c>
-      <c r="C46" s="9"/>
+      <c r="C46" s="9" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
       <c r="A47" s="7">
@@ -1059,7 +1070,9 @@
       <c r="B47" s="8">
         <v>45379</v>
       </c>
-      <c r="C47" s="9"/>
+      <c r="C47" s="9" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
       <c r="A48" s="7">
@@ -1068,7 +1081,9 @@
       <c r="B48" s="8">
         <v>45380</v>
       </c>
-      <c r="C48" s="9"/>
+      <c r="C48" s="9" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
       <c r="A49" s="7">
@@ -1077,7 +1092,9 @@
       <c r="B49" s="8">
         <v>45381</v>
       </c>
-      <c r="C49" s="9"/>
+      <c r="C49" s="9" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5">
       <c r="A50" s="7">
@@ -1086,7 +1103,9 @@
       <c r="B50" s="8">
         <v>45382</v>
       </c>
-      <c r="C50" s="9"/>
+      <c r="C50" s="9" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
       <c r="A51" s="7">

</xml_diff>

<commit_message>
New updates random file access
</commit_message>
<xml_diff>
--- a/2024FEB_M1.xlsx
+++ b/2024FEB_M1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
   <si>
     <t>S.N.</t>
   </si>
@@ -143,6 +143,12 @@
   </si>
   <si>
     <t>No class due to College Program</t>
+  </si>
+  <si>
+    <t>Random Access File</t>
+  </si>
+  <si>
+    <t>Ghode Jatra Holiday</t>
   </si>
 </sst>
 </file>
@@ -1189,7 +1195,9 @@
       <c r="B57" s="8">
         <v>45389</v>
       </c>
-      <c r="C57" s="9"/>
+      <c r="C57" s="9" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5">
       <c r="A58" s="7">
@@ -1198,7 +1206,9 @@
       <c r="B58" s="8">
         <v>45390</v>
       </c>
-      <c r="C58" s="9"/>
+      <c r="C58" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
       <c r="A59" s="7">

</xml_diff>

<commit_message>
Byte stream Class and Reading Writing Objects
</commit_message>
<xml_diff>
--- a/2024FEB_M1.xlsx
+++ b/2024FEB_M1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
   <si>
     <t>S.N.</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>Random file Access and Byte Stream Classes</t>
+  </si>
+  <si>
+    <t>Byte Stream Class, Reading and Writing Objects, Serializable</t>
   </si>
 </sst>
 </file>
@@ -572,7 +575,7 @@
   <cols>
     <col min="1" max="1" style="10" width="4.576428571428571" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="11" width="28.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="46.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="12" width="58.71928571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -1231,7 +1234,9 @@
       <c r="B60" s="8">
         <v>45392</v>
       </c>
-      <c r="C60" s="9"/>
+      <c r="C60" s="9" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
       <c r="A61" s="7">

</xml_diff>